<commit_message>
added more resumes and timesheet
</commit_message>
<xml_diff>
--- a/upload_timesheet.xlsx
+++ b/upload_timesheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>test_employee_id</t>
   </si>
@@ -22,9 +22,6 @@
     <t>filename</t>
   </si>
   <si>
-    <t>new_filename</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
@@ -125,6 +122,36 @@
   </si>
   <si>
     <t>15.docx</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>16.pdf</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>17.pdf</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>18.pdf</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>19.pdf</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>20.pdf</t>
   </si>
 </sst>
 </file>
@@ -204,8 +231,8 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -247,7 +274,7 @@
         <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4F818D"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="C0504D"/>
@@ -518,7 +545,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -528,8 +555,7 @@
     <col min="2" max="2" style="5" width="11.862142857142858" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="5" width="11.862142857142858" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="5" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="11.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -545,281 +571,308 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="16.5">
       <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4">
+      <c r="D2" s="3"/>
+      <c r="E2" s="4">
         <v>41.79</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="16.5">
       <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4">
         <v>29.88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="16.5">
       <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="4">
         <v>120.86</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="16.5">
       <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4">
         <v>41.78</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="16.5">
       <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4">
         <v>79.44</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="16.5">
       <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="C7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4">
         <v>31.87</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="16.5">
       <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="C8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4">
         <v>187.71</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="16.5">
       <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4">
         <v>79.92</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="16.5">
       <c r="A10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4">
         <v>48.95</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="16.5">
       <c r="A11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4">
         <v>49.82</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="16.5">
       <c r="A12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4">
+        <v>7</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4">
         <v>54.42</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="16.5">
       <c r="A13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="C13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4">
+        <v>7</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4">
         <v>101.57</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="16.5">
       <c r="A14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="C14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4">
         <v>187.12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="16.5">
       <c r="A15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="C15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4">
         <v>23.77</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="16.5">
       <c r="A16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4">
+        <v>20.07</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="16.5">
+      <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4">
-        <v>20.07</v>
+      <c r="B17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4">
+        <v>99.63</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="16.5">
+      <c r="A18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="4">
+        <v>71.28</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="16.5">
+      <c r="A19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4">
+        <v>59.6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="16.5">
+      <c r="A20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4">
+        <v>109.97</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="16.5">
+      <c r="A21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="4">
+        <v>61.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>